<commit_message>
Incluye pacientes hasta P29 sin P27 sin P09 Habiendo corregido grupos a Diciembre 2022
</commit_message>
<xml_diff>
--- a/AA_CODEX.xlsx
+++ b/AA_CODEX.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{63CC30C8-A0A1-4209-A215-8C277E1B08D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5B570D3-7FE2-124E-AE5B-A8F92378401E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28560" windowHeight="13905" firstSheet="4" activeTab="4" xr2:uid="{A22C7B05-6B0A-4116-A99A-60EDDEA67682}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28560" windowHeight="13900" xr2:uid="{A22C7B05-6B0A-4116-A99A-60EDDEA67682}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -42,11 +42,11 @@
   <commentList>
     <comment ref="B2" authorId="0" shapeId="0" xr:uid="{66C9BC75-6D95-457F-B28F-6603E41D1CFE}">
       <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t xml:space="preserve">[Comentario encadenado]
+Tu versión de Excel te permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
     segundos
-Reply:
+Respuesta:
     suma de los intentos
 </t>
       </text>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="431">
   <si>
     <t>CODIGO</t>
   </si>
@@ -608,7 +608,7 @@
     <t xml:space="preserve">LLamo el 22-ago-22 hablo con Margarita (mamá) me cuenta que es Macarena la que más dificultades tiene al parecer fueron episodios de VPPB(?) Agendo entrevista para ambas. OK correo entrevista inicial. LLamo el 2-sept-22 para confirmar participación y agendar horas, no contesta. </t>
   </si>
   <si>
-    <t>Revisar en Nucleo si ya concretamos</t>
+    <t>SIN NADA EN NUCLEO</t>
   </si>
   <si>
     <t>P16</t>
@@ -665,6 +665,9 @@
     <t>P18</t>
   </si>
   <si>
+    <t>Migraña Vestibular pura</t>
+  </si>
+  <si>
     <t>Nicole Thavata Zelada Iracheta</t>
   </si>
   <si>
@@ -735,9 +738,6 @@
   </si>
   <si>
     <t>P21</t>
-  </si>
-  <si>
-    <t>Vestibular-REVISAR MPPP</t>
   </si>
   <si>
     <t xml:space="preserve">Vertigo recurrente episodico - ¿Migraña vestibular? </t>
@@ -1357,7 +1357,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1382,7 +1382,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1396,7 +1396,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -1424,9 +1424,17 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="29">
+  <fills count="30">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1592,6 +1600,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFBFBFBF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1986,7 +2000,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="157">
+  <cellXfs count="158">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
@@ -2383,6 +2397,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="26" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2423,13 +2438,11 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Karen Villarroel" id="{60964397-01C8-4074-819B-979E0A14FF3E}" userId="0a6f7c1fb509c0b0" providerId="Windows Live"/>
-</personList>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2725,10 +2738,10 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="B2" dT="2022-11-13T00:28:20.51" personId="{60964397-01C8-4074-819B-979E0A14FF3E}" id="{66C9BC75-6D95-457F-B28F-6603E41D1CFE}">
+  <threadedComment ref="B2" dT="2022-11-13T00:28:20.51" personId="{00000000-0000-0000-0000-000000000000}" id="{66C9BC75-6D95-457F-B28F-6603E41D1CFE}">
     <text>segundos</text>
   </threadedComment>
-  <threadedComment ref="B2" dT="2022-11-13T01:17:34.71" personId="{60964397-01C8-4074-819B-979E0A14FF3E}" id="{4611028B-10C8-4770-81B7-7B212397757A}" parentId="{66C9BC75-6D95-457F-B28F-6603E41D1CFE}">
+  <threadedComment ref="B2" dT="2022-11-13T01:17:34.71" personId="{00000000-0000-0000-0000-000000000000}" id="{4611028B-10C8-4770-81B7-7B212397757A}" parentId="{66C9BC75-6D95-457F-B28F-6603E41D1CFE}">
     <text xml:space="preserve">suma de los intentos
 </text>
   </threadedComment>
@@ -2739,29 +2752,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F274FABB-DF5C-4F9E-B98F-F8DC866DADF5}">
   <dimension ref="A1:AG58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AG31" sqref="AG31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="7.85546875" style="73" customWidth="1"/>
-    <col min="3" max="5" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="7.83203125" style="73" customWidth="1"/>
+    <col min="3" max="5" width="15.6640625" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="27.42578125" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" customWidth="1"/>
-    <col min="11" max="12" width="17.7109375" customWidth="1"/>
-    <col min="13" max="13" width="22.140625" customWidth="1"/>
-    <col min="17" max="17" width="29.5703125" customWidth="1"/>
-    <col min="18" max="18" width="17.28515625" customWidth="1"/>
-    <col min="30" max="30" width="24.28515625" customWidth="1"/>
-    <col min="31" max="31" width="63.7109375" style="32" customWidth="1"/>
-    <col min="32" max="32" width="47.7109375" style="32" customWidth="1"/>
-    <col min="33" max="33" width="26.5703125" style="65" customWidth="1"/>
+    <col min="7" max="7" width="27.5" customWidth="1"/>
+    <col min="8" max="8" width="17.5" customWidth="1"/>
+    <col min="11" max="12" width="17.6640625" customWidth="1"/>
+    <col min="13" max="13" width="22.1640625" customWidth="1"/>
+    <col min="17" max="17" width="29.5" customWidth="1"/>
+    <col min="18" max="18" width="17.33203125" customWidth="1"/>
+    <col min="30" max="30" width="24.33203125" customWidth="1"/>
+    <col min="31" max="31" width="63.6640625" style="32" customWidth="1"/>
+    <col min="32" max="32" width="47.6640625" style="32" customWidth="1"/>
+    <col min="33" max="33" width="26.5" style="65" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="30">
+    <row r="1" spans="1:33" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2862,7 +2875,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:33">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>28</v>
       </c>
@@ -2924,7 +2937,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:33" ht="23.25">
+    <row r="3" spans="1:33" ht="29" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>39</v>
       </c>
@@ -3016,7 +3029,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:33" ht="23.25">
+    <row r="4" spans="1:33" ht="29" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>57</v>
       </c>
@@ -3106,7 +3119,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:33" ht="31.5" customHeight="1">
+    <row r="5" spans="1:33" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>67</v>
       </c>
@@ -3205,7 +3218,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:33" ht="35.25">
+    <row r="6" spans="1:33" ht="43" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>79</v>
       </c>
@@ -3296,7 +3309,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:33" ht="23.25">
+    <row r="7" spans="1:33" ht="29" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>89</v>
       </c>
@@ -3391,7 +3404,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:33" ht="35.25">
+    <row r="8" spans="1:33" ht="43" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>98</v>
       </c>
@@ -3480,7 +3493,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:33" ht="46.5">
+    <row r="9" spans="1:33" ht="57" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>108</v>
       </c>
@@ -3573,7 +3586,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:33" ht="46.5">
+    <row r="10" spans="1:33" ht="57" x14ac:dyDescent="0.2">
       <c r="A10" s="87" t="s">
         <v>119</v>
       </c>
@@ -3657,7 +3670,7 @@
       </c>
       <c r="AF10" s="67"/>
     </row>
-    <row r="11" spans="1:33" ht="23.25">
+    <row r="11" spans="1:33" ht="29" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>130</v>
       </c>
@@ -3665,7 +3678,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="D11" s="53">
         <v>23432</v>
@@ -3752,7 +3765,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="12" spans="1:33">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>139</v>
       </c>
@@ -3841,7 +3854,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="13" spans="1:33" ht="60.75">
+    <row r="13" spans="1:33" ht="48" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>147</v>
       </c>
@@ -3932,11 +3945,13 @@
         <v>155</v>
       </c>
     </row>
-    <row r="14" spans="1:33">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="B14" s="72"/>
+      <c r="B14" s="72">
+        <v>1</v>
+      </c>
       <c r="C14" s="55" t="s">
         <v>29</v>
       </c>
@@ -4021,11 +4036,13 @@
         <v>163</v>
       </c>
     </row>
-    <row r="15" spans="1:33">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="B15" s="69"/>
+      <c r="B15" s="69">
+        <v>1</v>
+      </c>
       <c r="C15" s="27" t="s">
         <v>40</v>
       </c>
@@ -4112,11 +4129,13 @@
         <v>163</v>
       </c>
     </row>
-    <row r="16" spans="1:33" ht="46.5">
+    <row r="16" spans="1:33" ht="57" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="B16" s="69"/>
+      <c r="B16" s="69">
+        <v>1</v>
+      </c>
       <c r="C16" s="27" t="s">
         <v>40</v>
       </c>
@@ -4197,16 +4216,20 @@
         <v>182</v>
       </c>
       <c r="AF16" s="67"/>
-      <c r="AG16" s="140" t="s">
+      <c r="AG16" s="150" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="17" spans="1:33" ht="23.25">
+    <row r="17" spans="1:33" ht="29" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="B17" s="69"/>
-      <c r="C17" s="55"/>
+      <c r="B17" s="69">
+        <v>1</v>
+      </c>
+      <c r="C17" s="55" t="s">
+        <v>29</v>
+      </c>
       <c r="D17" s="105">
         <v>34872</v>
       </c>
@@ -4286,11 +4309,13 @@
         <v>190</v>
       </c>
     </row>
-    <row r="18" spans="1:33" ht="46.5">
+    <row r="18" spans="1:33" ht="57" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="B18" s="69"/>
+      <c r="B18" s="69">
+        <v>1</v>
+      </c>
       <c r="C18" s="76" t="s">
         <v>40</v>
       </c>
@@ -4373,26 +4398,32 @@
       <c r="AF18" s="67" t="s">
         <v>200</v>
       </c>
-      <c r="AG18" s="140" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="19" spans="1:33">
+      <c r="AG18" s="65" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="B19" s="69"/>
-      <c r="C19" s="76"/>
+      <c r="B19" s="69">
+        <v>1</v>
+      </c>
+      <c r="C19" s="76" t="s">
+        <v>40</v>
+      </c>
       <c r="D19" s="75">
         <v>33967</v>
       </c>
       <c r="E19" s="84"/>
-      <c r="F19" s="56"/>
+      <c r="F19" s="56" t="s">
+        <v>202</v>
+      </c>
       <c r="G19" s="9" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="I19" s="9">
         <v>29</v>
@@ -4409,13 +4440,13 @@
       </c>
       <c r="N19" s="9"/>
       <c r="O19" s="9" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="P19" s="45">
         <v>932329343</v>
       </c>
       <c r="Q19" s="146" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="R19" s="60">
         <v>44819</v>
@@ -4427,7 +4458,7 @@
         <v>44838</v>
       </c>
       <c r="U19" s="12" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="V19" s="12" t="s">
         <v>105</v>
@@ -4436,7 +4467,7 @@
         <v>44838</v>
       </c>
       <c r="X19" s="13" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="Y19" s="43">
         <v>44875</v>
@@ -4455,18 +4486,20 @@
         <v>37</v>
       </c>
       <c r="AE19" s="31" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="AF19" s="67"/>
       <c r="AG19" s="141" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="20" spans="1:33">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="B20" s="101"/>
+        <v>211</v>
+      </c>
+      <c r="B20" s="101">
+        <v>1</v>
+      </c>
       <c r="C20" s="58" t="s">
         <v>40</v>
       </c>
@@ -4475,13 +4508,13 @@
       </c>
       <c r="E20" s="27"/>
       <c r="F20" s="27" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="I20" s="9">
         <v>30</v>
@@ -4498,13 +4531,13 @@
       </c>
       <c r="N20" s="9"/>
       <c r="O20" s="9" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="P20" s="45">
         <v>959440427</v>
       </c>
       <c r="Q20" s="146" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="R20" s="60">
         <v>44833</v>
@@ -4516,7 +4549,7 @@
         <v>44838</v>
       </c>
       <c r="U20" s="12" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="V20" s="12" t="s">
         <v>105</v>
@@ -4544,33 +4577,35 @@
         <v>37</v>
       </c>
       <c r="AE20" s="31" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="AF20" s="67"/>
       <c r="AG20" s="140" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="21" spans="1:33">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="B21" s="69"/>
+        <v>220</v>
+      </c>
+      <c r="B21" s="69">
+        <v>1</v>
+      </c>
       <c r="C21" s="27" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="D21" s="103">
         <v>33939</v>
       </c>
       <c r="E21" s="27"/>
       <c r="F21" s="27" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="I21" s="9">
         <v>30</v>
@@ -4587,13 +4622,13 @@
       </c>
       <c r="N21" s="9"/>
       <c r="O21" s="9" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="P21" s="45">
         <v>999362417</v>
       </c>
       <c r="Q21" s="146" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="R21" s="60">
         <v>44833</v>
@@ -4633,20 +4668,22 @@
         <v>37</v>
       </c>
       <c r="AE21" s="31" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="AF21" s="67"/>
       <c r="AG21" s="140" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="22" spans="1:33" ht="46.5">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" ht="43" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
-        <v>225</v>
-      </c>
-      <c r="B22" s="97"/>
+        <v>226</v>
+      </c>
+      <c r="B22" s="97">
+        <v>1</v>
+      </c>
       <c r="C22" s="61" t="s">
-        <v>226</v>
+        <v>58</v>
       </c>
       <c r="D22" s="102">
         <v>29848</v>
@@ -4731,11 +4768,13 @@
         <v>163</v>
       </c>
     </row>
-    <row r="23" spans="1:33">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A23" s="98" t="s">
         <v>236</v>
       </c>
-      <c r="B23" s="101"/>
+      <c r="B23" s="101">
+        <v>1</v>
+      </c>
       <c r="C23" s="99" t="s">
         <v>29</v>
       </c>
@@ -4805,11 +4844,13 @@
       <c r="AE23" s="31"/>
       <c r="AF23" s="67"/>
     </row>
-    <row r="24" spans="1:33" ht="23.25">
+    <row r="24" spans="1:33" ht="29" x14ac:dyDescent="0.2">
       <c r="A24" s="26" t="s">
         <v>242</v>
       </c>
-      <c r="B24" s="101"/>
+      <c r="B24" s="101">
+        <v>1</v>
+      </c>
       <c r="C24" s="58" t="s">
         <v>58</v>
       </c>
@@ -4888,13 +4929,15 @@
         <v>163</v>
       </c>
     </row>
-    <row r="25" spans="1:33" ht="24">
+    <row r="25" spans="1:33" ht="29" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="B25" s="97"/>
+      <c r="B25" s="97">
+        <v>1</v>
+      </c>
       <c r="C25" s="99" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="D25" s="107">
         <v>30800</v>
@@ -4966,11 +5009,13 @@
       </c>
       <c r="AF25" s="67"/>
     </row>
-    <row r="26" spans="1:33" ht="23.25">
+    <row r="26" spans="1:33" ht="29" x14ac:dyDescent="0.2">
       <c r="A26" s="26" t="s">
         <v>257</v>
       </c>
-      <c r="B26" s="69"/>
+      <c r="B26" s="69">
+        <v>1</v>
+      </c>
       <c r="C26" s="27" t="s">
         <v>40</v>
       </c>
@@ -5044,11 +5089,13 @@
       </c>
       <c r="AF26" s="67"/>
     </row>
-    <row r="27" spans="1:33">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A27" s="26" t="s">
         <v>265</v>
       </c>
-      <c r="B27" s="69"/>
+      <c r="B27" s="69">
+        <v>1</v>
+      </c>
       <c r="C27" s="27" t="s">
         <v>40</v>
       </c>
@@ -5122,7 +5169,7 @@
       </c>
       <c r="AF27" s="67"/>
     </row>
-    <row r="28" spans="1:33">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A28" s="26" t="s">
         <v>272</v>
       </c>
@@ -5180,11 +5227,13 @@
       <c r="AE28" s="31"/>
       <c r="AF28" s="67"/>
     </row>
-    <row r="29" spans="1:33" ht="29.25" customHeight="1">
+    <row r="29" spans="1:33" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="61" t="s">
         <v>275</v>
       </c>
-      <c r="B29" s="97"/>
+      <c r="B29" s="97">
+        <v>1</v>
+      </c>
       <c r="C29" s="61" t="s">
         <v>58</v>
       </c>
@@ -5262,11 +5311,13 @@
       </c>
       <c r="AF29" s="117"/>
     </row>
-    <row r="30" spans="1:33">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A30" s="26" t="s">
         <v>281</v>
       </c>
-      <c r="B30" s="69"/>
+      <c r="B30" s="69">
+        <v>1</v>
+      </c>
       <c r="C30" s="27" t="s">
         <v>58</v>
       </c>
@@ -5345,7 +5396,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="31" spans="1:33" ht="24">
+    <row r="31" spans="1:33" ht="29" x14ac:dyDescent="0.2">
       <c r="A31" s="26" t="s">
         <v>290</v>
       </c>
@@ -5431,7 +5482,7 @@
       </c>
       <c r="AF31" s="67"/>
     </row>
-    <row r="32" spans="1:33" ht="81">
+    <row r="32" spans="1:33" ht="99" x14ac:dyDescent="0.2">
       <c r="A32" s="26"/>
       <c r="B32" s="69"/>
       <c r="C32" s="76" t="s">
@@ -5479,7 +5530,7 @@
       </c>
       <c r="AF32" s="67"/>
     </row>
-    <row r="33" spans="1:32">
+    <row r="33" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A33" s="26"/>
       <c r="B33" s="100"/>
       <c r="C33" s="76" t="s">
@@ -5523,7 +5574,7 @@
       </c>
       <c r="AF33" s="67"/>
     </row>
-    <row r="34" spans="1:32" ht="26.25">
+    <row r="34" spans="1:32" ht="27" x14ac:dyDescent="0.2">
       <c r="A34" s="98"/>
       <c r="B34" s="97"/>
       <c r="C34" s="77" t="s">
@@ -5575,7 +5626,7 @@
       </c>
       <c r="AF34" s="67"/>
     </row>
-    <row r="35" spans="1:32">
+    <row r="35" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A35" s="98"/>
       <c r="B35" s="97"/>
       <c r="C35" s="77"/>
@@ -5617,7 +5668,7 @@
       </c>
       <c r="AF35" s="67"/>
     </row>
-    <row r="36" spans="1:32">
+    <row r="36" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A36" s="98"/>
       <c r="B36" s="109"/>
       <c r="C36" s="99"/>
@@ -5665,7 +5716,7 @@
       </c>
       <c r="AF36" s="67"/>
     </row>
-    <row r="37" spans="1:32">
+    <row r="37" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A37" s="26"/>
       <c r="B37" s="69"/>
       <c r="C37" s="27"/>
@@ -5699,7 +5750,7 @@
       <c r="AE37" s="31"/>
       <c r="AF37" s="67"/>
     </row>
-    <row r="38" spans="1:32">
+    <row r="38" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A38" s="26"/>
       <c r="B38" s="69"/>
       <c r="C38" s="27"/>
@@ -5733,7 +5784,7 @@
       <c r="AE38" s="31"/>
       <c r="AF38" s="67"/>
     </row>
-    <row r="39" spans="1:32">
+    <row r="39" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A39" s="26"/>
       <c r="B39" s="69"/>
       <c r="C39" s="27"/>
@@ -5767,7 +5818,7 @@
       <c r="AE39" s="31"/>
       <c r="AF39" s="67"/>
     </row>
-    <row r="40" spans="1:32">
+    <row r="40" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A40" s="26"/>
       <c r="B40" s="69"/>
       <c r="C40" s="27"/>
@@ -5801,7 +5852,7 @@
       <c r="AE40" s="31"/>
       <c r="AF40" s="67"/>
     </row>
-    <row r="41" spans="1:32">
+    <row r="41" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A41" s="26"/>
       <c r="B41" s="69"/>
       <c r="C41" s="27"/>
@@ -5835,7 +5886,7 @@
       <c r="AE41" s="31"/>
       <c r="AF41" s="67"/>
     </row>
-    <row r="42" spans="1:32">
+    <row r="42" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A42" s="26"/>
       <c r="B42" s="69"/>
       <c r="C42" s="27"/>
@@ -5869,7 +5920,7 @@
       <c r="AE42" s="31"/>
       <c r="AF42" s="67"/>
     </row>
-    <row r="43" spans="1:32">
+    <row r="43" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A43" s="26"/>
       <c r="B43" s="69"/>
       <c r="C43" s="27"/>
@@ -5903,7 +5954,7 @@
       <c r="AE43" s="31"/>
       <c r="AF43" s="67"/>
     </row>
-    <row r="44" spans="1:32">
+    <row r="44" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A44" s="26"/>
       <c r="B44" s="69"/>
       <c r="C44" s="27"/>
@@ -5937,7 +5988,7 @@
       <c r="AE44" s="31"/>
       <c r="AF44" s="67"/>
     </row>
-    <row r="45" spans="1:32">
+    <row r="45" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A45" s="26"/>
       <c r="B45" s="69"/>
       <c r="C45" s="27"/>
@@ -5971,7 +6022,7 @@
       <c r="AE45" s="31"/>
       <c r="AF45" s="67"/>
     </row>
-    <row r="46" spans="1:32">
+    <row r="46" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A46" s="26"/>
       <c r="B46" s="69"/>
       <c r="C46" s="27"/>
@@ -6005,7 +6056,7 @@
       <c r="AE46" s="31"/>
       <c r="AF46" s="67"/>
     </row>
-    <row r="47" spans="1:32">
+    <row r="47" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A47" s="26"/>
       <c r="B47" s="69"/>
       <c r="C47" s="27"/>
@@ -6039,7 +6090,7 @@
       <c r="AE47" s="31"/>
       <c r="AF47" s="67"/>
     </row>
-    <row r="48" spans="1:32">
+    <row r="48" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A48" s="26"/>
       <c r="B48" s="69"/>
       <c r="C48" s="27"/>
@@ -6073,7 +6124,7 @@
       <c r="AE48" s="31"/>
       <c r="AF48" s="67"/>
     </row>
-    <row r="49" spans="1:32">
+    <row r="49" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A49" s="26"/>
       <c r="B49" s="69"/>
       <c r="C49" s="27"/>
@@ -6107,7 +6158,7 @@
       <c r="AE49" s="31"/>
       <c r="AF49" s="67"/>
     </row>
-    <row r="50" spans="1:32">
+    <row r="50" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A50" s="26"/>
       <c r="B50" s="69"/>
       <c r="C50" s="27"/>
@@ -6141,7 +6192,7 @@
       <c r="AE50" s="31"/>
       <c r="AF50" s="67"/>
     </row>
-    <row r="51" spans="1:32">
+    <row r="51" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A51" s="26"/>
       <c r="B51" s="69"/>
       <c r="C51" s="27"/>
@@ -6175,7 +6226,7 @@
       <c r="AE51" s="31"/>
       <c r="AF51" s="67"/>
     </row>
-    <row r="52" spans="1:32">
+    <row r="52" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A52" s="26"/>
       <c r="B52" s="69"/>
       <c r="C52" s="27"/>
@@ -6209,7 +6260,7 @@
       <c r="AE52" s="31"/>
       <c r="AF52" s="67"/>
     </row>
-    <row r="53" spans="1:32">
+    <row r="53" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A53" s="26"/>
       <c r="B53" s="69"/>
       <c r="C53" s="27"/>
@@ -6243,7 +6294,7 @@
       <c r="AE53" s="31"/>
       <c r="AF53" s="67"/>
     </row>
-    <row r="54" spans="1:32">
+    <row r="54" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A54" s="26"/>
       <c r="B54" s="69"/>
       <c r="C54" s="27"/>
@@ -6277,7 +6328,7 @@
       <c r="AE54" s="31"/>
       <c r="AF54" s="67"/>
     </row>
-    <row r="55" spans="1:32">
+    <row r="55" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A55" s="26"/>
       <c r="B55" s="69"/>
       <c r="C55" s="27"/>
@@ -6311,7 +6362,7 @@
       <c r="AE55" s="31"/>
       <c r="AF55" s="67"/>
     </row>
-    <row r="56" spans="1:32">
+    <row r="56" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A56" s="26"/>
       <c r="B56" s="69"/>
       <c r="C56" s="27"/>
@@ -6345,7 +6396,7 @@
       <c r="AE56" s="31"/>
       <c r="AF56" s="67"/>
     </row>
-    <row r="57" spans="1:32">
+    <row r="57" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A57" s="26"/>
       <c r="B57" s="69"/>
       <c r="C57" s="27"/>
@@ -6379,7 +6430,7 @@
       <c r="AE57" s="31"/>
       <c r="AF57" s="67"/>
     </row>
-    <row r="58" spans="1:32">
+    <row r="58" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A58" s="26"/>
       <c r="B58" s="69"/>
       <c r="C58" s="27"/>
@@ -6448,33 +6499,33 @@
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
-      <c r="A1" s="153" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="154" t="s">
         <v>317</v>
       </c>
-      <c r="B1" s="154"/>
-      <c r="C1" s="154"/>
-      <c r="D1" s="154"/>
-      <c r="E1" s="154"/>
-      <c r="F1" s="154"/>
-      <c r="G1" s="154"/>
-      <c r="H1" s="154"/>
-      <c r="I1" s="154"/>
-      <c r="J1" s="154"/>
-      <c r="K1" s="154"/>
-      <c r="L1" s="154"/>
-      <c r="M1" s="155"/>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="B1" s="155"/>
+      <c r="C1" s="155"/>
+      <c r="D1" s="155"/>
+      <c r="E1" s="155"/>
+      <c r="F1" s="155"/>
+      <c r="G1" s="155"/>
+      <c r="H1" s="155"/>
+      <c r="I1" s="155"/>
+      <c r="J1" s="155"/>
+      <c r="K1" s="155"/>
+      <c r="L1" s="155"/>
+      <c r="M1" s="156"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="138" t="s">
         <v>105</v>
       </c>
@@ -6489,7 +6540,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="131" t="s">
         <v>319</v>
       </c>
@@ -6512,7 +6563,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="133" t="s">
         <v>326</v>
       </c>
@@ -6532,42 +6583,42 @@
         <v>329</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="153" t="s">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="154" t="s">
         <v>330</v>
       </c>
-      <c r="B9" s="154"/>
-      <c r="C9" s="154"/>
-      <c r="D9" s="154"/>
-      <c r="E9" s="154"/>
-      <c r="F9" s="154"/>
-      <c r="G9" s="154"/>
-      <c r="H9" s="154"/>
-      <c r="I9" s="154"/>
-      <c r="J9" s="154"/>
-      <c r="K9" s="154"/>
-      <c r="L9" s="154"/>
-      <c r="M9" s="155"/>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="150" t="s">
+      <c r="B9" s="155"/>
+      <c r="C9" s="155"/>
+      <c r="D9" s="155"/>
+      <c r="E9" s="155"/>
+      <c r="F9" s="155"/>
+      <c r="G9" s="155"/>
+      <c r="H9" s="155"/>
+      <c r="I9" s="155"/>
+      <c r="J9" s="155"/>
+      <c r="K9" s="155"/>
+      <c r="L9" s="155"/>
+      <c r="M9" s="156"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="151" t="s">
         <v>331</v>
       </c>
-      <c r="B11" s="151"/>
-      <c r="C11" s="151"/>
-      <c r="D11" s="151"/>
-      <c r="E11" s="152"/>
-      <c r="G11" s="150" t="s">
+      <c r="B11" s="152"/>
+      <c r="C11" s="152"/>
+      <c r="D11" s="152"/>
+      <c r="E11" s="153"/>
+      <c r="G11" s="151" t="s">
         <v>332</v>
       </c>
-      <c r="H11" s="151"/>
-      <c r="I11" s="151"/>
-      <c r="J11" s="151"/>
-      <c r="K11" s="151"/>
-      <c r="L11" s="151"/>
-      <c r="M11" s="152"/>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="H11" s="152"/>
+      <c r="I11" s="152"/>
+      <c r="J11" s="152"/>
+      <c r="K11" s="152"/>
+      <c r="L11" s="152"/>
+      <c r="M11" s="153"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="131" t="s">
         <v>333</v>
       </c>
@@ -6577,7 +6628,7 @@
       </c>
       <c r="M12" s="132"/>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="131" t="s">
         <v>335</v>
       </c>
@@ -6590,7 +6641,7 @@
       </c>
       <c r="M13" s="132"/>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="131" t="s">
         <v>337</v>
       </c>
@@ -6600,7 +6651,7 @@
       </c>
       <c r="M14" s="132"/>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="131" t="s">
         <v>14</v>
       </c>
@@ -6615,13 +6666,13 @@
       <c r="L15" s="134"/>
       <c r="M15" s="135"/>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="131" t="s">
         <v>16</v>
       </c>
       <c r="E16" s="132"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="133" t="s">
         <v>340</v>
       </c>
@@ -6630,77 +6681,77 @@
       <c r="D17" s="134"/>
       <c r="E17" s="135"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>355</v>
       </c>
@@ -6727,15 +6778,15 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" customWidth="1"/>
-    <col min="30" max="30" width="28.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" customWidth="1"/>
+    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5" customWidth="1"/>
+    <col min="30" max="30" width="28.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="24">
+    <row r="1" spans="1:32" ht="239" x14ac:dyDescent="0.2">
       <c r="A1" s="61"/>
       <c r="B1" s="61" t="s">
         <v>58</v>
@@ -6795,7 +6846,7 @@
       <c r="AE1" s="59"/>
       <c r="AF1" s="59"/>
     </row>
-    <row r="2" spans="1:32">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" s="59"/>
       <c r="B2" s="59"/>
       <c r="C2" s="59"/>
@@ -6837,7 +6888,7 @@
       <c r="AE2" s="59"/>
       <c r="AF2" s="59"/>
     </row>
-    <row r="4" spans="1:32" ht="36">
+    <row r="4" spans="1:32" ht="71" x14ac:dyDescent="0.2">
       <c r="A4" s="98"/>
       <c r="B4" s="97"/>
       <c r="C4" s="77" t="s">
@@ -6895,37 +6946,37 @@
       <c r="AE4" s="67"/>
       <c r="AF4" s="65"/>
     </row>
-    <row r="5" spans="1:32">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="D5" s="95"/>
       <c r="E5" s="95"/>
       <c r="F5" s="95"/>
     </row>
-    <row r="6" spans="1:32">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="D6" s="95"/>
       <c r="E6" s="95"/>
       <c r="F6" s="95"/>
     </row>
-    <row r="7" spans="1:32">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
       <c r="D7" s="96"/>
       <c r="E7" s="95"/>
       <c r="F7" s="95"/>
     </row>
-    <row r="8" spans="1:32">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="D8" s="95"/>
       <c r="E8" s="95"/>
       <c r="F8" s="95"/>
     </row>
-    <row r="9" spans="1:32">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
       <c r="D9" s="95"/>
       <c r="E9" s="95"/>
       <c r="F9" s="95"/>
     </row>
-    <row r="10" spans="1:32">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
       <c r="D10" s="95"/>
       <c r="E10" s="95"/>
       <c r="F10" s="95"/>
     </row>
-    <row r="11" spans="1:32">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
       <c r="D11" s="95"/>
       <c r="E11" s="95"/>
       <c r="F11" s="95"/>
@@ -6940,17 +6991,17 @@
   <dimension ref="A1:T69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S27" sqref="S27"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="48">
+    <row r="1" spans="1:20" ht="57" x14ac:dyDescent="0.2">
       <c r="A1" s="33" t="s">
         <v>372</v>
       </c>
@@ -7012,7 +7063,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="147" t="s">
         <v>28</v>
       </c>
@@ -7072,7 +7123,7 @@
       </c>
       <c r="T2" s="10"/>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="147" t="s">
         <v>39</v>
       </c>
@@ -7118,7 +7169,7 @@
       <c r="S3" s="41"/>
       <c r="T3" s="10"/>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="147" t="s">
         <v>57</v>
       </c>
@@ -7166,7 +7217,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="147" t="s">
         <v>67</v>
       </c>
@@ -7212,7 +7263,7 @@
       <c r="S5" s="41"/>
       <c r="T5" s="10"/>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="147" t="s">
         <v>79</v>
       </c>
@@ -7258,7 +7309,7 @@
       <c r="S6" s="41"/>
       <c r="T6" s="10"/>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="147" t="s">
         <v>89</v>
       </c>
@@ -7304,7 +7355,7 @@
       <c r="S7" s="41"/>
       <c r="T7" s="10"/>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="147" t="s">
         <v>98</v>
       </c>
@@ -7350,7 +7401,7 @@
       <c r="S8" s="41"/>
       <c r="T8" s="10"/>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="147" t="s">
         <v>108</v>
       </c>
@@ -7396,7 +7447,7 @@
       <c r="S9" s="41"/>
       <c r="T9" s="10"/>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="147" t="s">
         <v>119</v>
       </c>
@@ -7422,7 +7473,7 @@
       <c r="S10" s="129"/>
       <c r="T10" s="129"/>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="147" t="s">
         <v>130</v>
       </c>
@@ -7468,7 +7519,7 @@
       <c r="S11" s="41"/>
       <c r="T11" s="10"/>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="147" t="s">
         <v>139</v>
       </c>
@@ -7514,7 +7565,7 @@
       <c r="S12" s="41"/>
       <c r="T12" s="10"/>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="147" t="s">
         <v>147</v>
       </c>
@@ -7560,7 +7611,7 @@
       <c r="S13" s="41"/>
       <c r="T13" s="10"/>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="147" t="s">
         <v>156</v>
       </c>
@@ -7602,7 +7653,7 @@
       <c r="S14" s="41"/>
       <c r="T14" s="10"/>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="147" t="s">
         <v>164</v>
       </c>
@@ -7648,7 +7699,7 @@
       <c r="S15" s="41"/>
       <c r="T15" s="10"/>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" s="147" t="s">
         <v>174</v>
       </c>
@@ -7690,7 +7741,7 @@
       <c r="S16" s="41"/>
       <c r="T16" s="10"/>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="147" t="s">
         <v>184</v>
       </c>
@@ -7736,7 +7787,7 @@
       <c r="S17" s="41"/>
       <c r="T17" s="10"/>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" s="147" t="s">
         <v>191</v>
       </c>
@@ -7782,12 +7833,12 @@
       <c r="S18" s="41"/>
       <c r="T18" s="10"/>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" s="147" t="s">
         <v>201</v>
       </c>
       <c r="B19" s="149" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C19" s="10">
         <v>27</v>
@@ -7828,12 +7879,12 @@
       <c r="S19" s="41"/>
       <c r="T19" s="10"/>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" s="147" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B20" s="149" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C20" s="10">
         <v>30</v>
@@ -7874,12 +7925,12 @@
       <c r="S20" s="41"/>
       <c r="T20" s="10"/>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="147" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B21" s="149" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C21" s="10">
         <v>25</v>
@@ -7920,9 +7971,9 @@
       <c r="S21" s="41"/>
       <c r="T21" s="10"/>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" s="147" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B22" s="149" t="s">
         <v>229</v>
@@ -7966,7 +8017,7 @@
       <c r="S22" s="41"/>
       <c r="T22" s="10"/>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" s="147" t="s">
         <v>236</v>
       </c>
@@ -8012,7 +8063,7 @@
       <c r="S23" s="41"/>
       <c r="T23" s="10"/>
     </row>
-    <row r="24" spans="1:20">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" s="147" t="s">
         <v>242</v>
       </c>
@@ -8058,7 +8109,7 @@
       <c r="S24" s="41"/>
       <c r="T24" s="10"/>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" s="147" t="s">
         <v>250</v>
       </c>
@@ -8104,33 +8155,53 @@
       <c r="S25" s="41"/>
       <c r="T25" s="10"/>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" s="147" t="s">
         <v>257</v>
       </c>
       <c r="B26" s="149" t="s">
         <v>259</v>
       </c>
-      <c r="C26" s="10"/>
+      <c r="C26" s="10">
+        <v>29</v>
+      </c>
       <c r="D26" s="41"/>
-      <c r="E26" s="10"/>
+      <c r="E26" s="10">
+        <v>10</v>
+      </c>
       <c r="F26" s="41"/>
-      <c r="G26" s="10"/>
+      <c r="G26" s="10">
+        <v>10</v>
+      </c>
       <c r="H26" s="41"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
+      <c r="I26" s="10">
+        <v>0</v>
+      </c>
+      <c r="J26" s="10">
+        <v>26</v>
+      </c>
       <c r="K26" s="41"/>
-      <c r="L26" s="10"/>
-      <c r="M26" s="10"/>
+      <c r="L26" s="10">
+        <v>0</v>
+      </c>
+      <c r="M26" s="10">
+        <v>48</v>
+      </c>
       <c r="N26" s="41"/>
-      <c r="O26" s="10"/>
-      <c r="P26" s="10"/>
+      <c r="O26" s="10">
+        <v>10</v>
+      </c>
+      <c r="P26" s="10">
+        <v>9</v>
+      </c>
       <c r="Q26" s="41"/>
-      <c r="R26" s="10"/>
+      <c r="R26" s="10">
+        <v>34</v>
+      </c>
       <c r="S26" s="41"/>
       <c r="T26" s="10"/>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" s="147" t="s">
         <v>265</v>
       </c>
@@ -8176,7 +8247,7 @@
       <c r="S27" s="41"/>
       <c r="T27" s="10"/>
     </row>
-    <row r="28" spans="1:20">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" s="147" t="s">
         <v>272</v>
       </c>
@@ -8202,7 +8273,7 @@
       <c r="S28" s="41"/>
       <c r="T28" s="10"/>
     </row>
-    <row r="29" spans="1:20">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" s="147" t="s">
         <v>275</v>
       </c>
@@ -8248,7 +8319,7 @@
       <c r="S29" s="41"/>
       <c r="T29" s="10"/>
     </row>
-    <row r="30" spans="1:20">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" s="42" t="s">
         <v>281</v>
       </c>
@@ -8294,7 +8365,7 @@
       <c r="S30" s="41"/>
       <c r="T30" s="10"/>
     </row>
-    <row r="31" spans="1:20">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" s="42"/>
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
@@ -8316,7 +8387,7 @@
       <c r="S31" s="41"/>
       <c r="T31" s="10"/>
     </row>
-    <row r="32" spans="1:20">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" s="42"/>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
@@ -8338,7 +8409,7 @@
       <c r="S32" s="41"/>
       <c r="T32" s="10"/>
     </row>
-    <row r="33" spans="1:20">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33" s="42"/>
       <c r="B33" s="10"/>
       <c r="C33" s="10"/>
@@ -8360,7 +8431,7 @@
       <c r="S33" s="41"/>
       <c r="T33" s="10"/>
     </row>
-    <row r="34" spans="1:20">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34" s="42"/>
       <c r="B34" s="10"/>
       <c r="C34" s="10"/>
@@ -8382,7 +8453,7 @@
       <c r="S34" s="41"/>
       <c r="T34" s="10"/>
     </row>
-    <row r="35" spans="1:20">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" s="42"/>
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
@@ -8404,7 +8475,7 @@
       <c r="S35" s="41"/>
       <c r="T35" s="10"/>
     </row>
-    <row r="36" spans="1:20">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A36" s="42"/>
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
@@ -8426,7 +8497,7 @@
       <c r="S36" s="41"/>
       <c r="T36" s="10"/>
     </row>
-    <row r="37" spans="1:20">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37" s="42"/>
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
@@ -8448,7 +8519,7 @@
       <c r="S37" s="41"/>
       <c r="T37" s="10"/>
     </row>
-    <row r="38" spans="1:20">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" s="42"/>
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
@@ -8470,7 +8541,7 @@
       <c r="S38" s="41"/>
       <c r="T38" s="10"/>
     </row>
-    <row r="39" spans="1:20">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39" s="42"/>
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
@@ -8492,7 +8563,7 @@
       <c r="S39" s="41"/>
       <c r="T39" s="10"/>
     </row>
-    <row r="40" spans="1:20">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A40" s="42"/>
       <c r="B40" s="10"/>
       <c r="C40" s="10"/>
@@ -8514,7 +8585,7 @@
       <c r="S40" s="41"/>
       <c r="T40" s="10"/>
     </row>
-    <row r="41" spans="1:20">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A41" s="42"/>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
@@ -8536,7 +8607,7 @@
       <c r="S41" s="41"/>
       <c r="T41" s="10"/>
     </row>
-    <row r="42" spans="1:20">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A42" s="42"/>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
@@ -8558,7 +8629,7 @@
       <c r="S42" s="41"/>
       <c r="T42" s="10"/>
     </row>
-    <row r="43" spans="1:20">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43" s="42"/>
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
@@ -8580,7 +8651,7 @@
       <c r="S43" s="41"/>
       <c r="T43" s="10"/>
     </row>
-    <row r="44" spans="1:20">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A44" s="42"/>
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
@@ -8602,7 +8673,7 @@
       <c r="S44" s="41"/>
       <c r="T44" s="10"/>
     </row>
-    <row r="45" spans="1:20">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A45" s="42"/>
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
@@ -8624,7 +8695,7 @@
       <c r="S45" s="41"/>
       <c r="T45" s="10"/>
     </row>
-    <row r="46" spans="1:20">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A46" s="42"/>
       <c r="B46" s="10"/>
       <c r="C46" s="10"/>
@@ -8646,7 +8717,7 @@
       <c r="S46" s="41"/>
       <c r="T46" s="10"/>
     </row>
-    <row r="47" spans="1:20">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A47" s="42"/>
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
@@ -8668,7 +8739,7 @@
       <c r="S47" s="41"/>
       <c r="T47" s="10"/>
     </row>
-    <row r="48" spans="1:20">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A48" s="42"/>
       <c r="B48" s="10"/>
       <c r="C48" s="10"/>
@@ -8690,7 +8761,7 @@
       <c r="S48" s="41"/>
       <c r="T48" s="10"/>
     </row>
-    <row r="49" spans="1:20">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A49" s="42"/>
       <c r="B49" s="10"/>
       <c r="C49" s="10"/>
@@ -8712,7 +8783,7 @@
       <c r="S49" s="41"/>
       <c r="T49" s="10"/>
     </row>
-    <row r="50" spans="1:20">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A50" s="42"/>
       <c r="B50" s="10"/>
       <c r="C50" s="10"/>
@@ -8734,7 +8805,7 @@
       <c r="S50" s="41"/>
       <c r="T50" s="10"/>
     </row>
-    <row r="51" spans="1:20">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A51" s="42"/>
       <c r="B51" s="10"/>
       <c r="C51" s="10"/>
@@ -8756,7 +8827,7 @@
       <c r="S51" s="41"/>
       <c r="T51" s="10"/>
     </row>
-    <row r="52" spans="1:20">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A52" s="42"/>
       <c r="B52" s="10"/>
       <c r="C52" s="10"/>
@@ -8778,7 +8849,7 @@
       <c r="S52" s="41"/>
       <c r="T52" s="10"/>
     </row>
-    <row r="53" spans="1:20">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A53" s="42"/>
       <c r="B53" s="10"/>
       <c r="C53" s="10"/>
@@ -8800,7 +8871,7 @@
       <c r="S53" s="41"/>
       <c r="T53" s="10"/>
     </row>
-    <row r="54" spans="1:20">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A54" s="42"/>
       <c r="B54" s="10"/>
       <c r="C54" s="10"/>
@@ -8822,7 +8893,7 @@
       <c r="S54" s="41"/>
       <c r="T54" s="10"/>
     </row>
-    <row r="55" spans="1:20">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A55" s="42"/>
       <c r="B55" s="10"/>
       <c r="C55" s="10"/>
@@ -8844,7 +8915,7 @@
       <c r="S55" s="41"/>
       <c r="T55" s="10"/>
     </row>
-    <row r="56" spans="1:20">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A56" s="42"/>
       <c r="B56" s="10"/>
       <c r="C56" s="10"/>
@@ -8866,7 +8937,7 @@
       <c r="S56" s="41"/>
       <c r="T56" s="10"/>
     </row>
-    <row r="57" spans="1:20">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A57" s="42"/>
       <c r="B57" s="10"/>
       <c r="C57" s="10"/>
@@ -8888,7 +8959,7 @@
       <c r="S57" s="41"/>
       <c r="T57" s="10"/>
     </row>
-    <row r="58" spans="1:20">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A58" s="42"/>
       <c r="B58" s="10"/>
       <c r="C58" s="10"/>
@@ -8910,7 +8981,7 @@
       <c r="S58" s="41"/>
       <c r="T58" s="10"/>
     </row>
-    <row r="59" spans="1:20">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A59" s="42"/>
       <c r="B59" s="10"/>
       <c r="C59" s="10"/>
@@ -8932,7 +9003,7 @@
       <c r="S59" s="41"/>
       <c r="T59" s="10"/>
     </row>
-    <row r="60" spans="1:20">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A60" s="42"/>
       <c r="B60" s="10"/>
       <c r="C60" s="10"/>
@@ -8954,7 +9025,7 @@
       <c r="S60" s="41"/>
       <c r="T60" s="10"/>
     </row>
-    <row r="61" spans="1:20">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A61" s="42"/>
       <c r="B61" s="10"/>
       <c r="C61" s="10"/>
@@ -8976,7 +9047,7 @@
       <c r="S61" s="41"/>
       <c r="T61" s="10"/>
     </row>
-    <row r="62" spans="1:20">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A62" s="42"/>
       <c r="B62" s="10"/>
       <c r="C62" s="10"/>
@@ -8998,7 +9069,7 @@
       <c r="S62" s="41"/>
       <c r="T62" s="10"/>
     </row>
-    <row r="63" spans="1:20">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A63" s="42"/>
       <c r="B63" s="10"/>
       <c r="C63" s="10"/>
@@ -9020,7 +9091,7 @@
       <c r="S63" s="41"/>
       <c r="T63" s="10"/>
     </row>
-    <row r="64" spans="1:20">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A64" s="42"/>
       <c r="B64" s="10"/>
       <c r="C64" s="10"/>
@@ -9042,7 +9113,7 @@
       <c r="S64" s="41"/>
       <c r="T64" s="10"/>
     </row>
-    <row r="65" spans="1:20">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A65" s="42"/>
       <c r="B65" s="10"/>
       <c r="C65" s="10"/>
@@ -9064,7 +9135,7 @@
       <c r="S65" s="41"/>
       <c r="T65" s="10"/>
     </row>
-    <row r="66" spans="1:20">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A66" s="42"/>
       <c r="B66" s="10"/>
       <c r="C66" s="10"/>
@@ -9086,7 +9157,7 @@
       <c r="S66" s="41"/>
       <c r="T66" s="10"/>
     </row>
-    <row r="67" spans="1:20">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A67" s="42"/>
       <c r="B67" s="10"/>
       <c r="C67" s="10"/>
@@ -9108,7 +9179,7 @@
       <c r="S67" s="41"/>
       <c r="T67" s="10"/>
     </row>
-    <row r="68" spans="1:20">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A68" s="42"/>
       <c r="B68" s="10"/>
       <c r="C68" s="10"/>
@@ -9130,7 +9201,7 @@
       <c r="S68" s="41"/>
       <c r="T68" s="10"/>
     </row>
-    <row r="69" spans="1:20">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A69" s="42"/>
       <c r="B69" s="10"/>
       <c r="C69" s="10"/>
@@ -9161,83 +9232,82 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E734F7E-0347-4BF0-8C36-E23BB043549A}">
   <dimension ref="A1:Z60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="D7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z29" sqref="Z29"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Z28" sqref="Z28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="3" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="6" width="12.28515625" customWidth="1"/>
-    <col min="7" max="8" width="11.28515625" customWidth="1"/>
-    <col min="9" max="10" width="11.85546875" customWidth="1"/>
-    <col min="11" max="12" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="6" width="12.33203125" customWidth="1"/>
+    <col min="7" max="8" width="11.33203125" customWidth="1"/>
+    <col min="9" max="10" width="11.83203125" customWidth="1"/>
+    <col min="11" max="12" width="12.83203125" customWidth="1"/>
     <col min="13" max="14" width="12" customWidth="1"/>
-    <col min="15" max="16" width="11.85546875" customWidth="1"/>
-    <col min="17" max="18" width="11.5703125" customWidth="1"/>
-    <col min="19" max="20" width="11.42578125" customWidth="1"/>
-    <col min="21" max="22" width="11.28515625" customWidth="1"/>
-    <col min="23" max="23" width="12.140625" customWidth="1"/>
-    <col min="24" max="24" width="12.5703125" customWidth="1"/>
-    <col min="26" max="26" width="13.140625" customWidth="1"/>
+    <col min="15" max="16" width="11.83203125" customWidth="1"/>
+    <col min="17" max="20" width="11.5" customWidth="1"/>
+    <col min="21" max="22" width="11.33203125" customWidth="1"/>
+    <col min="23" max="23" width="12.1640625" customWidth="1"/>
+    <col min="24" max="24" width="12.5" customWidth="1"/>
+    <col min="26" max="26" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>372</v>
       </c>
-      <c r="B1" s="156" t="s">
+      <c r="B1" s="157" t="s">
         <v>387</v>
       </c>
-      <c r="C1" s="156"/>
-      <c r="D1" s="156" t="s">
+      <c r="C1" s="157"/>
+      <c r="D1" s="157" t="s">
         <v>388</v>
       </c>
-      <c r="E1" s="156"/>
-      <c r="F1" s="156" t="s">
+      <c r="E1" s="157"/>
+      <c r="F1" s="157" t="s">
         <v>389</v>
       </c>
-      <c r="G1" s="156"/>
-      <c r="H1" s="156" t="s">
+      <c r="G1" s="157"/>
+      <c r="H1" s="157" t="s">
         <v>390</v>
       </c>
-      <c r="I1" s="156"/>
-      <c r="J1" s="156" t="s">
+      <c r="I1" s="157"/>
+      <c r="J1" s="157" t="s">
         <v>391</v>
       </c>
-      <c r="K1" s="156"/>
-      <c r="L1" s="156" t="s">
+      <c r="K1" s="157"/>
+      <c r="L1" s="157" t="s">
         <v>392</v>
       </c>
-      <c r="M1" s="156"/>
-      <c r="N1" s="156" t="s">
+      <c r="M1" s="157"/>
+      <c r="N1" s="157" t="s">
         <v>393</v>
       </c>
-      <c r="O1" s="156"/>
-      <c r="P1" s="156" t="s">
+      <c r="O1" s="157"/>
+      <c r="P1" s="157" t="s">
         <v>394</v>
       </c>
-      <c r="Q1" s="156"/>
-      <c r="R1" s="156" t="s">
+      <c r="Q1" s="157"/>
+      <c r="R1" s="157" t="s">
         <v>395</v>
       </c>
-      <c r="S1" s="156"/>
-      <c r="T1" s="156" t="s">
+      <c r="S1" s="157"/>
+      <c r="T1" s="157" t="s">
         <v>396</v>
       </c>
-      <c r="U1" s="156"/>
-      <c r="V1" s="156" t="s">
+      <c r="U1" s="157"/>
+      <c r="V1" s="157" t="s">
         <v>397</v>
       </c>
-      <c r="W1" s="156"/>
-      <c r="X1" s="156" t="s">
+      <c r="W1" s="157"/>
+      <c r="X1" s="157" t="s">
         <v>398</v>
       </c>
-      <c r="Y1" s="156"/>
-    </row>
-    <row r="2" spans="1:26">
+      <c r="Y1" s="157"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B2" s="125" t="s">
         <v>399</v>
       </c>
@@ -9314,7 +9384,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="61" t="s">
         <v>28</v>
       </c>
@@ -9394,7 +9464,7 @@
         <v>4.1203703703703706E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="61" t="s">
         <v>39</v>
       </c>
@@ -9474,7 +9544,7 @@
         <v>5.5555555555555558E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="61" t="s">
         <v>57</v>
       </c>
@@ -9554,7 +9624,7 @@
         <v>1.0856481481481481E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="61" t="s">
         <v>67</v>
       </c>
@@ -9634,7 +9704,7 @@
         <v>1.0763888888888891E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="61" t="s">
         <v>79</v>
       </c>
@@ -9714,7 +9784,7 @@
         <v>9.6527777777777775E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="61" t="s">
         <v>89</v>
       </c>
@@ -9794,7 +9864,7 @@
         <v>7.1527777777777787E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="61" t="s">
         <v>98</v>
       </c>
@@ -9874,7 +9944,7 @@
         <v>8.4953703703703701E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="61" t="s">
         <v>108</v>
       </c>
@@ -9954,7 +10024,7 @@
         <v>6.053240740740741E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="123" t="s">
         <v>119</v>
       </c>
@@ -9984,7 +10054,7 @@
       <c r="Y11" s="124"/>
       <c r="Z11" s="124"/>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="61" t="s">
         <v>130</v>
       </c>
@@ -10064,7 +10134,7 @@
         <v>8.2638888888888883E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="61" t="s">
         <v>139</v>
       </c>
@@ -10144,7 +10214,7 @@
         <v>7.0254629629629634E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="61" t="s">
         <v>147</v>
       </c>
@@ -10224,7 +10294,7 @@
         <v>8.7152777777777784E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="61" t="s">
         <v>156</v>
       </c>
@@ -10304,7 +10374,7 @@
         <v>7.4537037037037028E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="61" t="s">
         <v>164</v>
       </c>
@@ -10384,7 +10454,7 @@
         <v>4.5138888888888893E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:26">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" s="61" t="s">
         <v>174</v>
       </c>
@@ -10464,7 +10534,7 @@
         <v>5.5324074074074069E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:26">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" s="61" t="s">
         <v>184</v>
       </c>
@@ -10544,7 +10614,7 @@
         <v>8.4837962962962966E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:26">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A19" s="61" t="s">
         <v>191</v>
       </c>
@@ -10624,7 +10694,7 @@
         <v>8.7847222222222233E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20" s="61" t="s">
         <v>201</v>
       </c>
@@ -10704,9 +10774,9 @@
         <v>6.6087962962962966E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:26">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21" s="61" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B21" s="59">
         <v>3</v>
@@ -10784,9 +10854,9 @@
         <v>5.9953703703703697E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:26">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A22" s="61" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B22" s="59">
         <v>2</v>
@@ -10864,9 +10934,9 @@
         <v>4.386574074074074E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:26">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" s="61" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B23" s="59">
         <v>2</v>
@@ -10944,7 +11014,7 @@
         <v>9.1435185185185178E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:26">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A24" s="61" t="s">
         <v>236</v>
       </c>
@@ -11024,7 +11094,7 @@
         <v>4.9768518518518521E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:26">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A25" s="61" t="s">
         <v>242</v>
       </c>
@@ -11109,7 +11179,7 @@
         <v>7.8819444444444432E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:26">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A26" s="61" t="s">
         <v>250</v>
       </c>
@@ -11194,37 +11264,89 @@
         <v>6.9328703703703696E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:26">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A27" s="61" t="s">
         <v>257</v>
       </c>
-      <c r="B27" s="59"/>
-      <c r="C27" s="59"/>
-      <c r="D27" s="59"/>
-      <c r="E27" s="59"/>
-      <c r="F27" s="59"/>
-      <c r="G27" s="59"/>
-      <c r="H27" s="59"/>
-      <c r="I27" s="59"/>
-      <c r="J27" s="59"/>
-      <c r="K27" s="59"/>
-      <c r="L27" s="59"/>
-      <c r="M27" s="59"/>
-      <c r="N27" s="59"/>
-      <c r="O27" s="59"/>
-      <c r="P27" s="59"/>
-      <c r="Q27" s="59"/>
-      <c r="R27" s="59"/>
-      <c r="S27" s="59"/>
-      <c r="T27" s="59"/>
-      <c r="U27" s="59"/>
-      <c r="V27" s="59"/>
-      <c r="W27" s="59"/>
-      <c r="X27" s="59"/>
-      <c r="Y27" s="59"/>
-      <c r="Z27" s="59"/>
-    </row>
-    <row r="28" spans="1:26">
+      <c r="B27" s="59">
+        <v>1</v>
+      </c>
+      <c r="C27" s="59">
+        <v>1</v>
+      </c>
+      <c r="D27" s="59">
+        <v>2</v>
+      </c>
+      <c r="E27" s="59">
+        <v>1</v>
+      </c>
+      <c r="F27" s="59">
+        <v>3</v>
+      </c>
+      <c r="G27" s="59">
+        <v>1</v>
+      </c>
+      <c r="H27" s="59">
+        <v>2</v>
+      </c>
+      <c r="I27" s="59">
+        <v>1</v>
+      </c>
+      <c r="J27" s="59">
+        <v>2</v>
+      </c>
+      <c r="K27" s="59">
+        <v>1</v>
+      </c>
+      <c r="L27" s="59">
+        <f>4+5</f>
+        <v>9</v>
+      </c>
+      <c r="M27" s="59">
+        <v>2</v>
+      </c>
+      <c r="N27" s="59">
+        <v>6</v>
+      </c>
+      <c r="O27" s="59">
+        <v>1</v>
+      </c>
+      <c r="P27" s="59">
+        <f>8+31</f>
+        <v>39</v>
+      </c>
+      <c r="Q27" s="59">
+        <v>2</v>
+      </c>
+      <c r="R27" s="59">
+        <v>10</v>
+      </c>
+      <c r="S27" s="59">
+        <v>1</v>
+      </c>
+      <c r="T27" s="59">
+        <v>3</v>
+      </c>
+      <c r="U27" s="59">
+        <v>1</v>
+      </c>
+      <c r="V27" s="59">
+        <v>6</v>
+      </c>
+      <c r="W27" s="59">
+        <v>1</v>
+      </c>
+      <c r="X27" s="59">
+        <v>74</v>
+      </c>
+      <c r="Y27" s="59">
+        <v>1</v>
+      </c>
+      <c r="Z27" s="122">
+        <v>3.9814814814814817E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A28" s="61" t="s">
         <v>265</v>
       </c>
@@ -11307,7 +11429,7 @@
         <v>6.1111111111111114E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:26">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A29" s="61" t="s">
         <v>272</v>
       </c>
@@ -11337,7 +11459,7 @@
       <c r="Y29" s="59"/>
       <c r="Z29" s="59"/>
     </row>
-    <row r="30" spans="1:26">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A30" s="61" t="s">
         <v>275</v>
       </c>
@@ -11419,7 +11541,7 @@
         <v>5.2546296296296299E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:26">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A31" s="61" t="s">
         <v>281</v>
       </c>
@@ -11504,7 +11626,7 @@
         <v>6.5624999999999998E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:26">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A32" s="61" t="s">
         <v>290</v>
       </c>
@@ -11534,7 +11656,7 @@
       <c r="Y32" s="59"/>
       <c r="Z32" s="59"/>
     </row>
-    <row r="33" spans="1:26">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A33" s="61" t="s">
         <v>403</v>
       </c>
@@ -11564,7 +11686,7 @@
       <c r="Y33" s="59"/>
       <c r="Z33" s="59"/>
     </row>
-    <row r="34" spans="1:26">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A34" s="61" t="s">
         <v>404</v>
       </c>
@@ -11594,7 +11716,7 @@
       <c r="Y34" s="59"/>
       <c r="Z34" s="59"/>
     </row>
-    <row r="35" spans="1:26">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A35" s="61" t="s">
         <v>405</v>
       </c>
@@ -11624,7 +11746,7 @@
       <c r="Y35" s="59"/>
       <c r="Z35" s="59"/>
     </row>
-    <row r="36" spans="1:26">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A36" s="61" t="s">
         <v>406</v>
       </c>
@@ -11654,7 +11776,7 @@
       <c r="Y36" s="59"/>
       <c r="Z36" s="59"/>
     </row>
-    <row r="37" spans="1:26">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A37" s="61" t="s">
         <v>407</v>
       </c>
@@ -11684,7 +11806,7 @@
       <c r="Y37" s="59"/>
       <c r="Z37" s="59"/>
     </row>
-    <row r="38" spans="1:26">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A38" s="61" t="s">
         <v>408</v>
       </c>
@@ -11714,7 +11836,7 @@
       <c r="Y38" s="59"/>
       <c r="Z38" s="59"/>
     </row>
-    <row r="39" spans="1:26">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A39" s="61" t="s">
         <v>409</v>
       </c>
@@ -11744,7 +11866,7 @@
       <c r="Y39" s="59"/>
       <c r="Z39" s="59"/>
     </row>
-    <row r="40" spans="1:26">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A40" s="61" t="s">
         <v>410</v>
       </c>
@@ -11774,7 +11896,7 @@
       <c r="Y40" s="59"/>
       <c r="Z40" s="59"/>
     </row>
-    <row r="41" spans="1:26">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A41" s="61" t="s">
         <v>411</v>
       </c>
@@ -11804,7 +11926,7 @@
       <c r="Y41" s="59"/>
       <c r="Z41" s="59"/>
     </row>
-    <row r="42" spans="1:26">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A42" s="61" t="s">
         <v>412</v>
       </c>
@@ -11834,7 +11956,7 @@
       <c r="Y42" s="59"/>
       <c r="Z42" s="59"/>
     </row>
-    <row r="43" spans="1:26">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A43" s="61" t="s">
         <v>413</v>
       </c>
@@ -11864,7 +11986,7 @@
       <c r="Y43" s="59"/>
       <c r="Z43" s="59"/>
     </row>
-    <row r="44" spans="1:26">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A44" s="61" t="s">
         <v>414</v>
       </c>
@@ -11894,7 +12016,7 @@
       <c r="Y44" s="59"/>
       <c r="Z44" s="59"/>
     </row>
-    <row r="45" spans="1:26">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A45" s="61" t="s">
         <v>415</v>
       </c>
@@ -11924,7 +12046,7 @@
       <c r="Y45" s="59"/>
       <c r="Z45" s="59"/>
     </row>
-    <row r="46" spans="1:26">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A46" s="61" t="s">
         <v>416</v>
       </c>
@@ -11954,7 +12076,7 @@
       <c r="Y46" s="59"/>
       <c r="Z46" s="59"/>
     </row>
-    <row r="47" spans="1:26">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A47" s="61" t="s">
         <v>417</v>
       </c>
@@ -11984,7 +12106,7 @@
       <c r="Y47" s="59"/>
       <c r="Z47" s="59"/>
     </row>
-    <row r="48" spans="1:26">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A48" s="61" t="s">
         <v>418</v>
       </c>
@@ -12014,7 +12136,7 @@
       <c r="Y48" s="59"/>
       <c r="Z48" s="59"/>
     </row>
-    <row r="49" spans="1:26">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A49" s="61" t="s">
         <v>419</v>
       </c>
@@ -12044,7 +12166,7 @@
       <c r="Y49" s="59"/>
       <c r="Z49" s="59"/>
     </row>
-    <row r="50" spans="1:26">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A50" s="61" t="s">
         <v>420</v>
       </c>
@@ -12074,7 +12196,7 @@
       <c r="Y50" s="59"/>
       <c r="Z50" s="59"/>
     </row>
-    <row r="51" spans="1:26">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A51" s="61" t="s">
         <v>421</v>
       </c>
@@ -12104,7 +12226,7 @@
       <c r="Y51" s="59"/>
       <c r="Z51" s="59"/>
     </row>
-    <row r="52" spans="1:26">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A52" s="61" t="s">
         <v>422</v>
       </c>
@@ -12134,7 +12256,7 @@
       <c r="Y52" s="59"/>
       <c r="Z52" s="59"/>
     </row>
-    <row r="53" spans="1:26">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A53" s="61" t="s">
         <v>423</v>
       </c>
@@ -12164,7 +12286,7 @@
       <c r="Y53" s="59"/>
       <c r="Z53" s="59"/>
     </row>
-    <row r="54" spans="1:26">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A54" s="61" t="s">
         <v>424</v>
       </c>
@@ -12194,7 +12316,7 @@
       <c r="Y54" s="59"/>
       <c r="Z54" s="59"/>
     </row>
-    <row r="55" spans="1:26">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A55" s="61" t="s">
         <v>425</v>
       </c>
@@ -12224,7 +12346,7 @@
       <c r="Y55" s="59"/>
       <c r="Z55" s="59"/>
     </row>
-    <row r="56" spans="1:26">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A56" s="61" t="s">
         <v>426</v>
       </c>
@@ -12254,7 +12376,7 @@
       <c r="Y56" s="59"/>
       <c r="Z56" s="59"/>
     </row>
-    <row r="57" spans="1:26">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A57" s="61" t="s">
         <v>427</v>
       </c>
@@ -12284,7 +12406,7 @@
       <c r="Y57" s="59"/>
       <c r="Z57" s="59"/>
     </row>
-    <row r="58" spans="1:26">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A58" s="61" t="s">
         <v>428</v>
       </c>
@@ -12314,7 +12436,7 @@
       <c r="Y58" s="59"/>
       <c r="Z58" s="59"/>
     </row>
-    <row r="59" spans="1:26">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A59" s="61" t="s">
         <v>429</v>
       </c>
@@ -12344,7 +12466,7 @@
       <c r="Y59" s="59"/>
       <c r="Z59" s="59"/>
     </row>
-    <row r="60" spans="1:26">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A60" s="61" t="s">
         <v>430</v>
       </c>

</xml_diff>

<commit_message>
Incluye pacientes hasta P29 sin P27 sin P09 Habiendo corregido grupos a Diciembre 2022 Revisión de Banish List Añadimos descriptor básico por grupos!
</commit_message>
<xml_diff>
--- a/AA_CODEX.xlsx
+++ b/AA_CODEX.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5B570D3-7FE2-124E-AE5B-A8F92378401E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{75C1626A-D8F3-244F-8473-5A4B6758C481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28560" windowHeight="13900" xr2:uid="{A22C7B05-6B0A-4116-A99A-60EDDEA67682}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="432">
   <si>
     <t>CODIGO</t>
   </si>
@@ -178,88 +178,88 @@
     <t>P02</t>
   </si>
   <si>
+    <t>MPPP</t>
+  </si>
+  <si>
+    <t>MV, VPPB</t>
+  </si>
+  <si>
+    <t>Migraña Vestibular; Vertigo Posicional</t>
+  </si>
+  <si>
+    <t>Rossana Fiorentino</t>
+  </si>
+  <si>
+    <t>8.896.452-7</t>
+  </si>
+  <si>
+    <t>Femenino</t>
+  </si>
+  <si>
+    <t>Si</t>
+  </si>
+  <si>
+    <t>C. Alemana</t>
+  </si>
+  <si>
+    <t>rossanafiorentino@gmail.com</t>
+  </si>
+  <si>
+    <t>8.45</t>
+  </si>
+  <si>
+    <t>9.30</t>
+  </si>
+  <si>
+    <t>Hayo y Rosario</t>
+  </si>
+  <si>
+    <t>11.00</t>
+  </si>
+  <si>
+    <t>15.00</t>
+  </si>
+  <si>
+    <t>16.00</t>
+  </si>
+  <si>
+    <t>Hayo, Karen y Felipe</t>
+  </si>
+  <si>
+    <t>// Caidas en SimianMaze --&gt; Bloque A en Trial 8 // Bloque C en Trial 3</t>
+  </si>
+  <si>
+    <t>P03</t>
+  </si>
+  <si>
+    <t>MPPP, MV</t>
+  </si>
+  <si>
+    <t>Migraña Vestibular; MPPP</t>
+  </si>
+  <si>
+    <t>Ximena Parra Vasquez</t>
+  </si>
+  <si>
+    <t>10.064.889-K</t>
+  </si>
+  <si>
+    <t>xparrav@yahoo.es</t>
+  </si>
+  <si>
+    <t>13.00</t>
+  </si>
+  <si>
+    <t>14.30</t>
+  </si>
+  <si>
+    <t>// Paciente No tolera RV, se suspende en Trial 4 de Bloque A en Modo RV</t>
+  </si>
+  <si>
+    <t>P04</t>
+  </si>
+  <si>
     <t>Vestibular</t>
-  </si>
-  <si>
-    <t>MV, VPPB</t>
-  </si>
-  <si>
-    <t>Migraña Vestibular; Vertigo Posicional</t>
-  </si>
-  <si>
-    <t>Rossana Fiorentino</t>
-  </si>
-  <si>
-    <t>8.896.452-7</t>
-  </si>
-  <si>
-    <t>Femenino</t>
-  </si>
-  <si>
-    <t>Si</t>
-  </si>
-  <si>
-    <t>C. Alemana</t>
-  </si>
-  <si>
-    <t>rossanafiorentino@gmail.com</t>
-  </si>
-  <si>
-    <t>8.45</t>
-  </si>
-  <si>
-    <t>9.30</t>
-  </si>
-  <si>
-    <t>Hayo y Rosario</t>
-  </si>
-  <si>
-    <t>11.00</t>
-  </si>
-  <si>
-    <t>15.00</t>
-  </si>
-  <si>
-    <t>16.00</t>
-  </si>
-  <si>
-    <t>Hayo, Karen y Felipe</t>
-  </si>
-  <si>
-    <t>// Caidas en SimianMaze --&gt; Bloque A en Trial 8 // Bloque C en Trial 3</t>
-  </si>
-  <si>
-    <t>P03</t>
-  </si>
-  <si>
-    <t>MPPP</t>
-  </si>
-  <si>
-    <t>MPPP, MV</t>
-  </si>
-  <si>
-    <t>Migraña Vestibular; MPPP</t>
-  </si>
-  <si>
-    <t>Ximena Parra Vasquez</t>
-  </si>
-  <si>
-    <t>10.064.889-K</t>
-  </si>
-  <si>
-    <t>xparrav@yahoo.es</t>
-  </si>
-  <si>
-    <t>13.00</t>
-  </si>
-  <si>
-    <t>14.30</t>
-  </si>
-  <si>
-    <t>// Paciente No tolera RV, se suspende en Trial 4 de Bloque A en Modo RV</t>
-  </si>
-  <si>
-    <t>P04</t>
   </si>
   <si>
     <t>VPPB, Vertigo visual</t>
@@ -904,6 +904,9 @@
   </si>
   <si>
     <t>P29</t>
+  </si>
+  <si>
+    <t>MPPP definitivo; Neuronitis vestibular post OTE</t>
   </si>
   <si>
     <t>Jorge Andrés Contreras Wachtendorff</t>
@@ -2753,8 +2756,8 @@
   <dimension ref="A1:AG58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3037,20 +3040,20 @@
         <v>1</v>
       </c>
       <c r="C4" s="94" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="G4" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="H4" s="9" t="s">
         <v>61</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>62</v>
       </c>
       <c r="I4" s="9">
         <v>57</v>
@@ -3075,7 +3078,7 @@
         <v>982934461</v>
       </c>
       <c r="Q4" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R4" s="19">
         <v>44708</v>
@@ -3085,7 +3088,7 @@
         <v>44708</v>
       </c>
       <c r="U4" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="V4" s="21" t="s">
         <v>51</v>
@@ -3094,7 +3097,7 @@
         <v>44708</v>
       </c>
       <c r="X4" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Y4" s="19">
         <v>44714</v>
@@ -3116,18 +3119,18 @@
       </c>
       <c r="AE4" s="31"/>
       <c r="AF4" s="67" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:33" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="71">
+        <v>1</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>67</v>
-      </c>
-      <c r="B5" s="71">
-        <v>1</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>40</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9" t="s">
@@ -3226,7 +3229,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="D6" s="27"/>
       <c r="E6" s="27" t="s">
@@ -3241,7 +3244,9 @@
       <c r="H6" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="I6" s="9"/>
+      <c r="I6" s="9">
+        <v>61</v>
+      </c>
       <c r="J6" s="9" t="s">
         <v>45</v>
       </c>
@@ -3317,7 +3322,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9" t="s">
@@ -3412,11 +3417,11 @@
         <v>1</v>
       </c>
       <c r="C8" s="94" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="F8" s="27" t="s">
         <v>99</v>
@@ -3501,7 +3506,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="9" t="s">
@@ -3592,7 +3597,7 @@
       </c>
       <c r="B10" s="88"/>
       <c r="C10" s="89" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="D10" s="89"/>
       <c r="E10" s="89"/>
@@ -3678,7 +3683,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="D11" s="53">
         <v>23432</v>
@@ -3773,7 +3778,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="D12" s="27"/>
       <c r="E12" s="27" t="s">
@@ -3862,7 +3867,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="94" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="D13" s="53">
         <v>24116</v>
@@ -4044,7 +4049,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="D15" s="53">
         <v>24398</v>
@@ -4137,7 +4142,7 @@
         <v>1</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="D16" s="104">
         <v>37621</v>
@@ -4317,7 +4322,7 @@
         <v>1</v>
       </c>
       <c r="C18" s="76" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="D18" s="75">
         <v>26700</v>
@@ -4410,7 +4415,7 @@
         <v>1</v>
       </c>
       <c r="C19" s="76" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="D19" s="75">
         <v>33967</v>
@@ -4501,7 +4506,7 @@
         <v>1</v>
       </c>
       <c r="C20" s="58" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="D20" s="103">
         <v>33696</v>
@@ -4592,7 +4597,7 @@
         <v>1</v>
       </c>
       <c r="C21" s="27" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="D21" s="103">
         <v>33939</v>
@@ -4683,7 +4688,7 @@
         <v>1</v>
       </c>
       <c r="C22" s="61" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="D22" s="102">
         <v>29848</v>
@@ -4731,7 +4736,7 @@
         <v>44854</v>
       </c>
       <c r="U22" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="V22" s="12" t="s">
         <v>105</v>
@@ -4852,7 +4857,7 @@
         <v>1</v>
       </c>
       <c r="C24" s="58" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="D24" s="103">
         <v>44165</v>
@@ -4937,7 +4942,7 @@
         <v>1</v>
       </c>
       <c r="C25" s="99" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="D25" s="107">
         <v>30800</v>
@@ -5017,7 +5022,7 @@
         <v>1</v>
       </c>
       <c r="C26" s="27" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="D26" s="103">
         <v>31010</v>
@@ -5097,7 +5102,7 @@
         <v>1</v>
       </c>
       <c r="C27" s="27" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="D27" s="103">
         <v>28102</v>
@@ -5235,7 +5240,7 @@
         <v>1</v>
       </c>
       <c r="C29" s="61" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="D29" s="118">
         <v>27019</v>
@@ -5279,7 +5284,7 @@
         <v>44882</v>
       </c>
       <c r="U29" s="112" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="V29" s="12" t="s">
         <v>105</v>
@@ -5319,18 +5324,20 @@
         <v>1</v>
       </c>
       <c r="C30" s="27" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="D30" s="53">
         <v>24488</v>
       </c>
-      <c r="E30" s="27"/>
+      <c r="E30" s="27" t="s">
+        <v>282</v>
+      </c>
       <c r="F30" s="27"/>
       <c r="G30" s="9" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="I30" s="9">
         <v>55</v>
@@ -5345,23 +5352,23 @@
       </c>
       <c r="N30" s="9"/>
       <c r="O30" s="9" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="P30" s="45">
         <v>992311317</v>
       </c>
       <c r="Q30" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="R30" s="46" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="S30" s="11"/>
       <c r="T30" s="43">
         <v>44895</v>
       </c>
       <c r="U30" s="12" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="V30" s="12" t="s">
         <v>105</v>
@@ -5389,35 +5396,35 @@
         <v>23</v>
       </c>
       <c r="AE30" s="31" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="AF30" s="67"/>
       <c r="AG30" s="65" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="31" spans="1:33" ht="29" x14ac:dyDescent="0.2">
       <c r="A31" s="26" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B31" s="69"/>
       <c r="C31" s="27" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="D31" s="53">
         <v>21473</v>
       </c>
       <c r="E31" s="27" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="F31" s="27" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="H31" s="9" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="I31" s="9">
         <v>64</v>
@@ -5428,17 +5435,17 @@
       <c r="K31" s="10"/>
       <c r="L31" s="10"/>
       <c r="M31" s="10" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="N31" s="9"/>
       <c r="O31" s="9" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="P31" s="45">
         <v>95764981</v>
       </c>
       <c r="Q31" s="59" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="R31" s="60">
         <v>44888</v>
@@ -5450,7 +5457,7 @@
         <v>44909</v>
       </c>
       <c r="U31" s="12" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="V31" s="12" t="s">
         <v>105</v>
@@ -5478,7 +5485,7 @@
         <v>241</v>
       </c>
       <c r="AE31" s="31" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="AF31" s="67"/>
     </row>
@@ -5486,13 +5493,13 @@
       <c r="A32" s="26"/>
       <c r="B32" s="69"/>
       <c r="C32" s="76" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="D32" s="54"/>
       <c r="E32" s="85"/>
       <c r="F32" s="77"/>
       <c r="G32" s="10" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="H32" s="9"/>
       <c r="I32" s="9">
@@ -5508,7 +5515,7 @@
         <v>953001359</v>
       </c>
       <c r="Q32" s="64" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="R32" s="10"/>
       <c r="S32" s="11"/>
@@ -5523,10 +5530,10 @@
       <c r="AB32" s="15"/>
       <c r="AC32" s="15"/>
       <c r="AD32" s="28" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="AE32" s="31" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="AF32" s="67"/>
     </row>
@@ -5534,13 +5541,13 @@
       <c r="A33" s="26"/>
       <c r="B33" s="100"/>
       <c r="C33" s="76" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="D33" s="54"/>
       <c r="E33" s="85"/>
       <c r="F33" s="78"/>
       <c r="G33" s="9" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="H33" s="9"/>
       <c r="I33" s="9"/>
@@ -5552,7 +5559,7 @@
       <c r="O33" s="9"/>
       <c r="P33" s="10"/>
       <c r="Q33" s="49" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="R33" s="10"/>
       <c r="S33" s="11"/>
@@ -5567,10 +5574,10 @@
       <c r="AB33" s="15"/>
       <c r="AC33" s="15"/>
       <c r="AD33" s="28" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="AE33" s="17" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="AF33" s="67"/>
     </row>
@@ -5584,7 +5591,7 @@
       <c r="E34" s="79"/>
       <c r="F34" s="29"/>
       <c r="G34" s="9" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="H34" s="9"/>
       <c r="I34" s="76">
@@ -5597,14 +5604,14 @@
       <c r="L34" s="46"/>
       <c r="M34" s="10"/>
       <c r="N34" s="30" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="O34" s="9"/>
       <c r="P34" s="45">
         <v>982105605</v>
       </c>
       <c r="Q34" s="63" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="R34" s="46"/>
       <c r="S34" s="11"/>
@@ -5619,10 +5626,10 @@
       <c r="AB34" s="15"/>
       <c r="AC34" s="15"/>
       <c r="AD34" s="28" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="AE34" s="17" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="AF34" s="67"/>
     </row>
@@ -5634,7 +5641,7 @@
       <c r="E35" s="79"/>
       <c r="F35" s="29"/>
       <c r="G35" s="9" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="H35" s="9"/>
       <c r="I35" s="76"/>
@@ -5661,10 +5668,10 @@
       <c r="AB35" s="15"/>
       <c r="AC35" s="15"/>
       <c r="AD35" s="28" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="AE35" s="17" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="AF35" s="67"/>
     </row>
@@ -5675,10 +5682,10 @@
       <c r="D36" s="99"/>
       <c r="E36" s="86"/>
       <c r="F36" s="56" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="H36" s="9"/>
       <c r="I36" s="76"/>
@@ -5694,7 +5701,7 @@
         <v>996413604</v>
       </c>
       <c r="Q36" s="54" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="R36" s="46"/>
       <c r="S36" s="11"/>
@@ -5709,10 +5716,10 @@
       <c r="AB36" s="15"/>
       <c r="AC36" s="15"/>
       <c r="AD36" s="28" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="AE36" s="31" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="AF36" s="67"/>
     </row>
@@ -6510,7 +6517,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="154" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B1" s="155"/>
       <c r="C1" s="155"/>
@@ -6537,55 +6544,55 @@
       </c>
       <c r="G3" s="137"/>
       <c r="H3" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="131" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B4" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C4" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D4" s="132" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="F4" s="131" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="G4" s="132" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="H4" s="44" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="133" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B5" s="134" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C5" s="134" t="s">
+        <v>328</v>
+      </c>
+      <c r="D5" s="135" t="s">
         <v>327</v>
       </c>
-      <c r="D5" s="135" t="s">
-        <v>326</v>
-      </c>
       <c r="F5" s="133" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="G5" s="135" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="154" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B9" s="155"/>
       <c r="C9" s="155"/>
@@ -6602,14 +6609,14 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="151" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B11" s="152"/>
       <c r="C11" s="152"/>
       <c r="D11" s="152"/>
       <c r="E11" s="153"/>
       <c r="G11" s="151" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="H11" s="152"/>
       <c r="I11" s="152"/>
@@ -6620,34 +6627,34 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="131" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="E12" s="132"/>
       <c r="G12" s="131" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="M12" s="132"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="131" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="E13" s="132"/>
       <c r="G13" s="131" t="s">
         <v>105</v>
       </c>
       <c r="H13" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="M13" s="132"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="131" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="E14" s="132"/>
       <c r="G14" s="131" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="M14" s="132"/>
     </row>
@@ -6657,7 +6664,7 @@
       </c>
       <c r="E15" s="132"/>
       <c r="G15" s="133" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="H15" s="134"/>
       <c r="I15" s="134"/>
@@ -6674,7 +6681,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="133" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B17" s="134"/>
       <c r="C17" s="134"/>
@@ -6683,77 +6690,77 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
   </sheetData>
@@ -6789,17 +6796,17 @@
     <row r="1" spans="1:32" ht="239" x14ac:dyDescent="0.2">
       <c r="A1" s="61"/>
       <c r="B1" s="61" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="C1" s="82">
         <v>26831</v>
       </c>
       <c r="D1" s="61"/>
       <c r="E1" s="54" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="F1" s="54" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="G1" s="54">
         <v>49</v>
@@ -6812,16 +6819,16 @@
         <v>123</v>
       </c>
       <c r="K1" s="54" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="L1" s="54" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="M1" s="110" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="N1" s="59" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="O1" s="110"/>
       <c r="P1" s="111"/>
@@ -6836,10 +6843,10 @@
       <c r="Y1" s="115"/>
       <c r="Z1" s="115"/>
       <c r="AA1" s="116" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="AB1" s="117" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="AC1" s="117"/>
       <c r="AD1" s="59"/>
@@ -6852,7 +6859,7 @@
       <c r="C2" s="59"/>
       <c r="D2" s="59"/>
       <c r="E2" s="54" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="F2" s="59"/>
       <c r="G2" s="59"/>
@@ -6865,7 +6872,7 @@
         <v>73387793</v>
       </c>
       <c r="N2" s="59" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="O2" s="59"/>
       <c r="P2" s="59"/>
@@ -6881,7 +6888,7 @@
       <c r="Z2" s="59"/>
       <c r="AA2" s="59"/>
       <c r="AB2" s="59" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="AC2" s="59"/>
       <c r="AD2" s="59"/>
@@ -6899,13 +6906,13 @@
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="27" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="I4" s="76">
         <v>42</v>
@@ -6917,13 +6924,13 @@
       </c>
       <c r="M4" s="9"/>
       <c r="N4" s="9" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="O4" s="45">
         <v>966471982</v>
       </c>
       <c r="P4" s="54" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="Q4" s="46"/>
       <c r="R4" s="11"/>
@@ -6938,10 +6945,10 @@
       <c r="AA4" s="15"/>
       <c r="AB4" s="15"/>
       <c r="AC4" s="28" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="AD4" s="31" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="AE4" s="67"/>
       <c r="AF4" s="65"/>
@@ -7003,64 +7010,64 @@
   <sheetData>
     <row r="1" spans="1:20" ht="57" x14ac:dyDescent="0.2">
       <c r="A1" s="33" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B1" s="34" t="s">
         <v>6</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="E1" s="36" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="F1" s="36" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="G1" s="36" t="s">
+        <v>378</v>
+      </c>
+      <c r="H1" s="36" t="s">
         <v>377</v>
       </c>
-      <c r="H1" s="36" t="s">
-        <v>376</v>
-      </c>
       <c r="I1" s="37" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="J1" s="37" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="K1" s="37" t="s">
+        <v>381</v>
+      </c>
+      <c r="L1" s="37" t="s">
+        <v>382</v>
+      </c>
+      <c r="M1" s="37" t="s">
         <v>380</v>
       </c>
-      <c r="L1" s="37" t="s">
+      <c r="N1" s="37" t="s">
         <v>381</v>
       </c>
-      <c r="M1" s="37" t="s">
-        <v>379</v>
-      </c>
-      <c r="N1" s="37" t="s">
-        <v>380</v>
-      </c>
       <c r="O1" s="38" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="P1" s="38" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="Q1" s="121" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="R1" s="121" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="S1" s="39" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="T1" s="40" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
@@ -7174,7 +7181,7 @@
         <v>57</v>
       </c>
       <c r="B4" s="149" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" s="10">
         <v>26</v>
@@ -7214,12 +7221,12 @@
       </c>
       <c r="S4" s="41"/>
       <c r="T4" s="10" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="147" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" s="149" t="s">
         <v>70</v>
@@ -8324,7 +8331,7 @@
         <v>281</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C30" s="10">
         <v>27</v>
@@ -9256,132 +9263,132 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B1" s="157" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C1" s="157"/>
       <c r="D1" s="157" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="E1" s="157"/>
       <c r="F1" s="157" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="G1" s="157"/>
       <c r="H1" s="157" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="I1" s="157"/>
       <c r="J1" s="157" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="K1" s="157"/>
       <c r="L1" s="157" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="M1" s="157"/>
       <c r="N1" s="157" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="O1" s="157"/>
       <c r="P1" s="157" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="Q1" s="157"/>
       <c r="R1" s="157" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="S1" s="157"/>
       <c r="T1" s="157" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="U1" s="157"/>
       <c r="V1" s="157" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="W1" s="157"/>
       <c r="X1" s="157" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="Y1" s="157"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B2" s="125" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C2" s="125" t="s">
+        <v>401</v>
+      </c>
+      <c r="D2" s="125" t="s">
         <v>400</v>
       </c>
-      <c r="D2" s="125" t="s">
-        <v>399</v>
-      </c>
       <c r="E2" s="125" t="s">
+        <v>401</v>
+      </c>
+      <c r="F2" s="125" t="s">
         <v>400</v>
       </c>
-      <c r="F2" s="125" t="s">
-        <v>399</v>
-      </c>
       <c r="G2" s="125" t="s">
+        <v>401</v>
+      </c>
+      <c r="H2" s="125" t="s">
         <v>400</v>
       </c>
-      <c r="H2" s="125" t="s">
-        <v>399</v>
-      </c>
       <c r="I2" s="125" t="s">
+        <v>401</v>
+      </c>
+      <c r="J2" s="125" t="s">
         <v>400</v>
       </c>
-      <c r="J2" s="125" t="s">
-        <v>399</v>
-      </c>
       <c r="K2" s="125" t="s">
+        <v>401</v>
+      </c>
+      <c r="L2" s="125" t="s">
         <v>400</v>
       </c>
-      <c r="L2" s="125" t="s">
-        <v>399</v>
-      </c>
       <c r="M2" s="125" t="s">
+        <v>401</v>
+      </c>
+      <c r="N2" s="125" t="s">
         <v>400</v>
       </c>
-      <c r="N2" s="125" t="s">
-        <v>399</v>
-      </c>
       <c r="O2" s="125" t="s">
+        <v>401</v>
+      </c>
+      <c r="P2" s="125" t="s">
         <v>400</v>
       </c>
-      <c r="P2" s="125" t="s">
-        <v>399</v>
-      </c>
       <c r="Q2" s="125" t="s">
+        <v>401</v>
+      </c>
+      <c r="R2" s="125" t="s">
         <v>400</v>
       </c>
-      <c r="R2" s="125" t="s">
-        <v>399</v>
-      </c>
       <c r="S2" s="125" t="s">
+        <v>401</v>
+      </c>
+      <c r="T2" s="125" t="s">
         <v>400</v>
       </c>
-      <c r="T2" s="125" t="s">
-        <v>399</v>
-      </c>
       <c r="U2" s="125" t="s">
+        <v>401</v>
+      </c>
+      <c r="V2" s="125" t="s">
         <v>400</v>
       </c>
-      <c r="V2" s="125" t="s">
-        <v>399</v>
-      </c>
       <c r="W2" s="125" t="s">
+        <v>401</v>
+      </c>
+      <c r="X2" s="125" t="s">
         <v>400</v>
       </c>
-      <c r="X2" s="125" t="s">
-        <v>399</v>
-      </c>
       <c r="Y2" s="127" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="Z2" s="126" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
@@ -9526,7 +9533,7 @@
         <v>20</v>
       </c>
       <c r="U4" s="59" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="V4" s="59">
         <v>5</v>
@@ -9626,7 +9633,7 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="61" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" s="59">
         <v>3</v>
@@ -9766,7 +9773,7 @@
         <v>24</v>
       </c>
       <c r="U7" s="59" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="V7" s="59">
         <v>6</v>
@@ -9926,7 +9933,7 @@
         <v>20</v>
       </c>
       <c r="U9" s="59" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="V9" s="59">
         <v>32</v>
@@ -10104,7 +10111,7 @@
         <v>60</v>
       </c>
       <c r="Q12" s="59" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="R12" s="59">
         <v>20</v>
@@ -10264,7 +10271,7 @@
         <v>20</v>
       </c>
       <c r="Q14" s="59" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="R14" s="59">
         <v>8</v>
@@ -10338,7 +10345,7 @@
         <v>16</v>
       </c>
       <c r="O15" s="59" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="P15" s="59">
         <v>5</v>
@@ -10356,7 +10363,7 @@
         <v>8</v>
       </c>
       <c r="U15" s="59" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="V15" s="59">
         <v>10</v>
@@ -10516,7 +10523,7 @@
         <v>27</v>
       </c>
       <c r="U17" s="59" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="V17" s="59">
         <v>5</v>
@@ -10528,7 +10535,7 @@
         <v>15</v>
       </c>
       <c r="Y17" s="59" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="Z17" s="122">
         <v>5.5324074074074069E-3</v>
@@ -10608,7 +10615,7 @@
         <v>25</v>
       </c>
       <c r="Y18" s="59" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="Z18" s="122">
         <v>8.4837962962962966E-3</v>
@@ -10996,7 +11003,7 @@
         <v>80</v>
       </c>
       <c r="U23" s="59" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="V23" s="59">
         <v>5</v>
@@ -11628,7 +11635,7 @@
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A32" s="61" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B32" s="59"/>
       <c r="C32" s="59"/>
@@ -11658,7 +11665,7 @@
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A33" s="61" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B33" s="59"/>
       <c r="C33" s="59"/>
@@ -11688,7 +11695,7 @@
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A34" s="61" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B34" s="59"/>
       <c r="C34" s="59"/>
@@ -11718,7 +11725,7 @@
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A35" s="61" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B35" s="59"/>
       <c r="C35" s="59"/>
@@ -11748,7 +11755,7 @@
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A36" s="61" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B36" s="59"/>
       <c r="C36" s="59"/>
@@ -11778,7 +11785,7 @@
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A37" s="61" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B37" s="59"/>
       <c r="C37" s="59"/>
@@ -11808,7 +11815,7 @@
     </row>
     <row r="38" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A38" s="61" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B38" s="59"/>
       <c r="C38" s="59"/>
@@ -11838,7 +11845,7 @@
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A39" s="61" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B39" s="59"/>
       <c r="C39" s="59"/>
@@ -11868,7 +11875,7 @@
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A40" s="61" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B40" s="59"/>
       <c r="C40" s="59"/>
@@ -11898,7 +11905,7 @@
     </row>
     <row r="41" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A41" s="61" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B41" s="59"/>
       <c r="C41" s="59"/>
@@ -11928,7 +11935,7 @@
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A42" s="61" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B42" s="59"/>
       <c r="C42" s="59"/>
@@ -11958,7 +11965,7 @@
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A43" s="61" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B43" s="59"/>
       <c r="C43" s="59"/>
@@ -11988,7 +11995,7 @@
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A44" s="61" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B44" s="59"/>
       <c r="C44" s="59"/>
@@ -12018,7 +12025,7 @@
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A45" s="61" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="B45" s="59"/>
       <c r="C45" s="59"/>
@@ -12048,7 +12055,7 @@
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A46" s="61" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B46" s="59"/>
       <c r="C46" s="59"/>
@@ -12078,7 +12085,7 @@
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A47" s="61" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B47" s="59"/>
       <c r="C47" s="59"/>
@@ -12108,7 +12115,7 @@
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A48" s="61" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B48" s="59"/>
       <c r="C48" s="59"/>
@@ -12138,7 +12145,7 @@
     </row>
     <row r="49" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A49" s="61" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B49" s="59"/>
       <c r="C49" s="59"/>
@@ -12168,7 +12175,7 @@
     </row>
     <row r="50" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A50" s="61" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B50" s="59"/>
       <c r="C50" s="59"/>
@@ -12198,7 +12205,7 @@
     </row>
     <row r="51" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A51" s="61" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B51" s="59"/>
       <c r="C51" s="59"/>
@@ -12228,7 +12235,7 @@
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A52" s="61" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B52" s="59"/>
       <c r="C52" s="59"/>
@@ -12258,7 +12265,7 @@
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A53" s="61" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B53" s="59"/>
       <c r="C53" s="59"/>
@@ -12288,7 +12295,7 @@
     </row>
     <row r="54" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A54" s="61" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B54" s="59"/>
       <c r="C54" s="59"/>
@@ -12318,7 +12325,7 @@
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A55" s="61" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B55" s="59"/>
       <c r="C55" s="59"/>
@@ -12348,7 +12355,7 @@
     </row>
     <row r="56" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A56" s="61" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B56" s="59"/>
       <c r="C56" s="59"/>
@@ -12378,7 +12385,7 @@
     </row>
     <row r="57" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A57" s="61" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B57" s="59"/>
       <c r="C57" s="59"/>
@@ -12408,7 +12415,7 @@
     </row>
     <row r="58" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A58" s="61" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B58" s="59"/>
       <c r="C58" s="59"/>
@@ -12438,7 +12445,7 @@
     </row>
     <row r="59" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A59" s="61" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B59" s="59"/>
       <c r="C59" s="59"/>
@@ -12468,7 +12475,7 @@
     </row>
     <row r="60" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A60" s="61" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B60" s="59"/>
       <c r="C60" s="59"/>

</xml_diff>

<commit_message>
Avanzando con LSL decripting Analizando marcadores
Avancé fuerte con Temás de analisis en RV
Y ahora estamos un test-Run confiable de análisis de los marcadores.
</commit_message>
<xml_diff>
--- a/AA_CODEX.xlsx
+++ b/AA_CODEX.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E217CD9-869E-7F4C-94AA-0D10959E6738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBDD46E8-D758-D746-9EA8-FD2DA481DB55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28560" windowHeight="13900" xr2:uid="{A22C7B05-6B0A-4116-A99A-60EDDEA67682}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="448">
   <si>
     <t>CODIGO</t>
   </si>
@@ -2471,10 +2471,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
@@ -2786,9 +2782,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F274FABB-DF5C-4F9E-B98F-F8DC866DADF5}">
   <dimension ref="A1:AK52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D48" sqref="D48"/>
+      <selection pane="topRight" activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5923,7 +5919,7 @@
       </c>
       <c r="B32" s="64"/>
       <c r="C32" s="51" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D32" s="141">
         <v>27638</v>
@@ -6284,7 +6280,9 @@
         <v>332</v>
       </c>
       <c r="B36" s="64"/>
-      <c r="C36" s="25"/>
+      <c r="C36" s="25" t="s">
+        <v>67</v>
+      </c>
       <c r="D36" s="49">
         <v>30037</v>
       </c>

</xml_diff>